<commit_message>
VCE scenario policy file updates
</commit_message>
<xml_diff>
--- a/InputData/elec/RQSD/RPS Qualifying Source Definitions.xlsx
+++ b/InputData/elec/RQSD/RPS Qualifying Source Definitions.xlsx
@@ -1,22 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI - units progress\InputData\elec\RQSD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\RMI\Virginia\Virginia_Model\InputData\elec\RQSD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CA0129-D0F4-4D71-82E9-197CE9BB327D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="24915" windowHeight="11565"/>
+    <workbookView xWindow="15270" yWindow="435" windowWidth="13230" windowHeight="13515" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="RQSD-BRQSD" sheetId="2" r:id="rId2"/>
     <sheet name="RQSD-RQSD" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -122,7 +133,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -271,6 +282,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -306,6 +334,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -481,27 +526,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="84.59765625" customWidth="1"/>
+    <col min="2" max="2" width="84.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,55 +554,55 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -569,23 +614,182 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <f>B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.59765625" customWidth="1"/>
-    <col min="2" max="2" width="22.86328125" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -593,7 +797,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -601,7 +805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -609,7 +813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -617,7 +821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -625,7 +829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -633,7 +837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -641,7 +845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -649,7 +853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -657,7 +861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -665,7 +869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -673,7 +877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -681,7 +885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -690,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -698,7 +902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -706,7 +910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -714,171 +918,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
       <c r="B17">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:B17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="24.59765625" customWidth="1"/>
-    <col min="2" max="2" width="22.86328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13">
-        <f>B2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>